<commit_message>
Updated Semis, resolved a conflict
</commit_message>
<xml_diff>
--- a/Data/Semiconductors.xlsx
+++ b/Data/Semiconductors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="BJT" sheetId="1" r:id="rId1"/>
@@ -233,8 +233,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -511,13 +539,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated lines in semis
</commit_message>
<xml_diff>
--- a/Data/Semiconductors.xlsx
+++ b/Data/Semiconductors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BJT" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
   <si>
     <t>Part Number</t>
   </si>
@@ -93,9 +93,6 @@
     <t>30uA</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>15pF</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>1N4007-T</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Rectifier Diode, 1A @ 1.1Vf, 1000Vrrm, DO-41</t>
   </si>
   <si>
@@ -172,6 +166,336 @@
   </si>
   <si>
     <t>Features</t>
+  </si>
+  <si>
+    <t>Small Signal</t>
+  </si>
+  <si>
+    <t>DO-35</t>
+  </si>
+  <si>
+    <t>0.3A</t>
+  </si>
+  <si>
+    <t>1V</t>
+  </si>
+  <si>
+    <t>5uA</t>
+  </si>
+  <si>
+    <t>100V</t>
+  </si>
+  <si>
+    <t>4.0pF</t>
+  </si>
+  <si>
+    <t>50V</t>
+  </si>
+  <si>
+    <t>1000V</t>
+  </si>
+  <si>
+    <t>BJT-0002</t>
+  </si>
+  <si>
+    <t>BJT-0003</t>
+  </si>
+  <si>
+    <t>BJT-0004</t>
+  </si>
+  <si>
+    <t>BJT-0005</t>
+  </si>
+  <si>
+    <t>BJT-0006</t>
+  </si>
+  <si>
+    <t>BJT-0007</t>
+  </si>
+  <si>
+    <t>BJT-0008</t>
+  </si>
+  <si>
+    <t>BJT-0009</t>
+  </si>
+  <si>
+    <t>BJT-0010</t>
+  </si>
+  <si>
+    <t>BJT-0011</t>
+  </si>
+  <si>
+    <t>BJT-0012</t>
+  </si>
+  <si>
+    <t>BJT-0013</t>
+  </si>
+  <si>
+    <t>BJT-0014</t>
+  </si>
+  <si>
+    <t>BJT-0015</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>MPSA18</t>
+  </si>
+  <si>
+    <t>NPN Vceo=45V, Ic=200mA, hfe=1150@10mA</t>
+  </si>
+  <si>
+    <t>NPN Darlington</t>
+  </si>
+  <si>
+    <t>MPSA14</t>
+  </si>
+  <si>
+    <t>NPN Darlington Vceo=30V, Ic=1.2A, hfe=10K@10mA</t>
+  </si>
+  <si>
+    <t>PNP Darlington</t>
+  </si>
+  <si>
+    <t>MPSA63</t>
+  </si>
+  <si>
+    <t>PNP Darlington Vceo=-30V, Ic=-500mA, hfe=5k@10mA</t>
+  </si>
+  <si>
+    <t>MPSA64</t>
+  </si>
+  <si>
+    <t>PNP Darlington Vceo=-30V, Ic=-500mA, hfe=10K@10mA</t>
+  </si>
+  <si>
+    <t>PNP</t>
+  </si>
+  <si>
+    <t>2n5087</t>
+  </si>
+  <si>
+    <t>PNP Vceo=50V, Ic=50mA, hfe=250@10mA</t>
+  </si>
+  <si>
+    <t>2N5088</t>
+  </si>
+  <si>
+    <t>NPN Vceo=30V, Ic=50mA, hfe=300@10mA</t>
+  </si>
+  <si>
+    <t>2N5089</t>
+  </si>
+  <si>
+    <t>NPN Vceo=25V, Ic=50mA, hfe=400@10mA</t>
+  </si>
+  <si>
+    <t>2n3904</t>
+  </si>
+  <si>
+    <t>NPN Vceo=40V, Ic=200mA, hfe=100@10mA</t>
+  </si>
+  <si>
+    <t>2n2222</t>
+  </si>
+  <si>
+    <t>NPN Vceo=40V, Ic=1A, hfe=75@10mA</t>
+  </si>
+  <si>
+    <t>2n3906</t>
+  </si>
+  <si>
+    <t>PNP Vceo=-40V, Ic=-200mA, hfe=100@10mA</t>
+  </si>
+  <si>
+    <t>2n4401</t>
+  </si>
+  <si>
+    <t>NPN Vceo=40V, Ic=600mA, hfe=80@10mA</t>
+  </si>
+  <si>
+    <t>2n4402</t>
+  </si>
+  <si>
+    <t>PNP Vceo=-40V, Ic=-600mA, hfe=50@10mA</t>
+  </si>
+  <si>
+    <t>2n4403</t>
+  </si>
+  <si>
+    <t>PNP Vceo=-40V, Ic=-600mA, hfe=100@10mA</t>
+  </si>
+  <si>
+    <t>BC550</t>
+  </si>
+  <si>
+    <t>NPN Vceo=45V, Ic=100mA, hfe=110@2mA</t>
+  </si>
+  <si>
+    <t>BC560</t>
+  </si>
+  <si>
+    <t>PNP Vceo=-45V, Ic=100mA, hfe=110@2mA</t>
+  </si>
+  <si>
+    <t>JFET</t>
+  </si>
+  <si>
+    <t>2N5457</t>
+  </si>
+  <si>
+    <t>N-JFET Vds=25V, Id=10mA, Vgs=-2.5V</t>
+  </si>
+  <si>
+    <t>N-JFET</t>
+  </si>
+  <si>
+    <t>2n5458</t>
+  </si>
+  <si>
+    <t>N-JFET Vds=25V, Id=10mA, Vgs=-3.5V</t>
+  </si>
+  <si>
+    <t>2n5459</t>
+  </si>
+  <si>
+    <t>N-FET Vds=25V, Id=10mA, Vgs=-4.5V</t>
+  </si>
+  <si>
+    <t>2n5460</t>
+  </si>
+  <si>
+    <t>P-FET Vds=40V, Id=10mA, Vgs=0.5V to 4V</t>
+  </si>
+  <si>
+    <t>P-JFET</t>
+  </si>
+  <si>
+    <t>2n5461</t>
+  </si>
+  <si>
+    <t>P-FET Vds=40V, Id=10mA, Vgs=0.8V to 4.5V</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>N-FET Vds=40V, Id=50mA, Vgs=-0.3V to -1.5V</t>
+  </si>
+  <si>
+    <t>J202</t>
+  </si>
+  <si>
+    <t>N-FET Vds=40V, Id=50mA, Vgs=-0.8V to -4V</t>
+  </si>
+  <si>
+    <t>MMBFJ201</t>
+  </si>
+  <si>
+    <t>MOSFET</t>
+  </si>
+  <si>
+    <t>2n7000</t>
+  </si>
+  <si>
+    <t>N-MOSFET Vds=60V, Id=200mA, Vgs=2.1V, Rds=1.2ohms</t>
+  </si>
+  <si>
+    <t>N-MOSFET</t>
+  </si>
+  <si>
+    <t>2n7002</t>
+  </si>
+  <si>
+    <t>N-MOSFET Vds=60V, Id=115mA, Vgs=2.1V , Rds=1.2ohms</t>
+  </si>
+  <si>
+    <t>J111</t>
+  </si>
+  <si>
+    <t>J112</t>
+  </si>
+  <si>
+    <t>J113</t>
+  </si>
+  <si>
+    <t>2n5484</t>
+  </si>
+  <si>
+    <t>2n5485</t>
+  </si>
+  <si>
+    <t>2n5486</t>
+  </si>
+  <si>
+    <t>BS170</t>
+  </si>
+  <si>
+    <t>Obsolete Low Noise, High Gain, Use MMBT5089</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Obsolete High Current Gain, up to 1A collector use MMBTA14</t>
+  </si>
+  <si>
+    <t>Obsolete High Current Gain, up to 800ma collector, use MMBTA63</t>
+  </si>
+  <si>
+    <t>JFET-0001</t>
+  </si>
+  <si>
+    <t>JFET-0002</t>
+  </si>
+  <si>
+    <t>JFET-0003</t>
+  </si>
+  <si>
+    <t>JFET-0004</t>
+  </si>
+  <si>
+    <t>JFET-0005</t>
+  </si>
+  <si>
+    <t>JFET-0006</t>
+  </si>
+  <si>
+    <t>JFET-0007</t>
+  </si>
+  <si>
+    <t>JFET-0008</t>
+  </si>
+  <si>
+    <t>JFET-0009</t>
+  </si>
+  <si>
+    <t>JFET-0010</t>
+  </si>
+  <si>
+    <t>JFET-0011</t>
+  </si>
+  <si>
+    <t>JFET-0012</t>
+  </si>
+  <si>
+    <t>JFET-0013</t>
+  </si>
+  <si>
+    <t>JFET-0014</t>
+  </si>
+  <si>
+    <t>MFET-0001</t>
+  </si>
+  <si>
+    <t>MFET-0002</t>
+  </si>
+  <si>
+    <t>MFET-0003</t>
   </si>
 </sst>
 </file>
@@ -537,15 +861,730 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,21 +1644,232 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -683,79 +1933,59 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -766,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -793,25 +2023,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -838,10 +2068,10 @@
         <v>10</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>11</v>
@@ -870,10 +2100,10 @@
     </row>
     <row r="2" spans="1:35" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>19</v>
@@ -888,19 +2118,19 @@
         <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O2" s="3" t="b">
         <v>0</v>
@@ -912,67 +2142,97 @@
         <v>18</v>
       </c>
       <c r="R2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:35" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:35" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="K4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:35" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>
@@ -987,34 +2247,34 @@
         <v>22</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="R5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U5" s="4"/>
       <c r="Y5" s="4"/>

</xml_diff>